<commit_message>
Commit 2; added more features; modified look and feel
</commit_message>
<xml_diff>
--- a/RootCauseAnalyzer/processed_defects.xlsx
+++ b/RootCauseAnalyzer/processed_defects.xlsx
@@ -575,7 +575,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>The most probable root cause is a compatibility or configuration issue between the Alaska Payments application and the Citrix environment, possibly triggered by an overly sensitive antivirus software. Refreshing the application likely resets the session or bypasses the temporary glitch causing the black screen.</t>
+          <t>The most probable root cause is an issue with the Alaska Payments application interface or compatibility within the Citrix environment, potentially triggered by recent updates or changes in software configurations, which was temporarily resolved by refreshing the application but may need a permanent fix for underlying compatibility or update issues.</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>The most probable root cause of the iCargo system running extremely slow was a problem within the iCargo network infrastructure, possibly due to network congestion or malfunctioning network hardware/software.</t>
+          <t>The most probable root cause is a network performance issue or congestion within the iCargo system's network infrastructure, leading to slow system response times and subsequent backups.</t>
         </is>
       </c>
     </row>

</xml_diff>